<commit_message>
Initial commit: Add Excel, HTML, images and PowerShell script
</commit_message>
<xml_diff>
--- a/skill_transfer_db.xlsx
+++ b/skill_transfer_db.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\logi_dx_transfer_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6AC6768-8330-4F2B-90EC-067D97A5316D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4203509-5AAC-4838-A976-A35342AA4165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6997F564-F219-4A2E-B5AC-9B2E50119CF6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5654B169-6ECA-45E6-B5BA-B1561B058AF5}"/>
   </bookViews>
   <sheets>
-    <sheet name="SkillTransfer" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>セクション</t>
   </si>
@@ -39,7 +39,7 @@
     <t>背景・課題</t>
   </si>
   <si>
-    <t>初期は手書きの出荷明細作成、品番のExcel入力といった手作業中心の業務運用...</t>
+    <t>初期は手書きの出荷明細作成、品番のExcel入力といった手作業中心の業務運用業務の属人化・ヒューマンエラー・在庫管理の精度低下が課題</t>
   </si>
   <si>
     <t>実施内容①</t>
@@ -51,22 +51,22 @@
     <t>実施内容②</t>
   </si>
   <si>
-    <t>Notionで誰でも在庫を確認できるダッシュボード構築</t>
+    <t>Notionで誰でも在庫を確認できるボタン付きダッシュボード構築</t>
   </si>
   <si>
     <t>成果</t>
   </si>
   <si>
-    <t>作業時間を約70%削減、在庫の透明性向上</t>
+    <t>出荷登録の作業時間を約70%削減、データの抜け漏れ解消、在庫の透明性向上</t>
   </si>
   <si>
     <t>② 繊維工場への物流業務委託時の構築支援</t>
   </si>
   <si>
-    <t>百貨店コードをGASで自動生成</t>
-  </si>
-  <si>
-    <t>値札データ→SATO機器へ印刷（GAS）</t>
+    <t>百貨店コードをGASで自動生成（命名規則化）</t>
+  </si>
+  <si>
+    <t>値札データ自動生成→SATO機器へ印刷（GAS）</t>
   </si>
   <si>
     <t>実施内容③</t>
@@ -78,61 +78,64 @@
     <t>実施内容④</t>
   </si>
   <si>
-    <t>LINE BOTでオーダー受付・転記</t>
-  </si>
-  <si>
-    <t>業務効率化、注文負荷軽減</t>
-  </si>
-  <si>
-    <t>③ 生産管理・原価管理の可視化支援</t>
+    <t>店舗からのオーダーをLINE BOTで受付・自動転記（GAS連携）</t>
+  </si>
+  <si>
+    <t>出荷準備業務の大幅効率化、LINEでの注文により業務負荷を軽減</t>
+  </si>
+  <si>
+    <t>③ 生産管理・原価管理の可視化支援（Notion）</t>
   </si>
   <si>
     <t>背景</t>
   </si>
   <si>
-    <t>Excel管理の限界（漏れ・見落とし）</t>
-  </si>
-  <si>
-    <t>Excelの変更を検知しNotion DB反映</t>
-  </si>
-  <si>
-    <t>原価・納期変更をリアルタイム可視化</t>
-  </si>
-  <si>
-    <t>情報連携が円滑に、月次作成半減</t>
-  </si>
-  <si>
-    <t>④ スキルトランスファー</t>
+    <t>Excel中心の管理で更新漏れ・重複入力・見落としリスク</t>
+  </si>
+  <si>
+    <t>現状のExcel入力を維持しつつ、GASで変更を検知</t>
+  </si>
+  <si>
+    <t>Notion DBにリアルタイム反映し、原価・納品タイミングを視覚化</t>
+  </si>
+  <si>
+    <t>データ履歴を記録、過去変更も追跡可</t>
+  </si>
+  <si>
+    <t>原価や納期変更の即時可視化、関係部署間の情報連携がスムーズに、月次資料作成を半減化</t>
+  </si>
+  <si>
+    <t>④ スキルトランスファー（技術移転）対応</t>
   </si>
   <si>
     <t>内容①</t>
   </si>
   <si>
-    <t>操作マニュアル、動画作成</t>
+    <t>GAS・Notion等の操作マニュアル作成</t>
   </si>
   <si>
     <t>内容②</t>
   </si>
   <si>
-    <t>対面/動画でのレクチャー実施</t>
+    <t>担当者向けレクチャー／動画 or 対面での説明会実施</t>
   </si>
   <si>
     <t>内容③</t>
   </si>
   <si>
-    <t>システム構成図・API連携図の作成</t>
+    <t>システム構成図やAPI連携図の作成</t>
   </si>
   <si>
     <t>内容④</t>
   </si>
   <si>
-    <t>チェックリスト整備</t>
-  </si>
-  <si>
-    <t>使用技術・ツール</t>
-  </si>
-  <si>
-    <t>GAS、Notion API、Python、LINE BOT、SATOプリンタ、Slack通知</t>
+    <t>日常業務へ落とし込むチェックリスト整備</t>
+  </si>
+  <si>
+    <t>使用技術・ツール一覧</t>
+  </si>
+  <si>
+    <t>Google Apps Script（GAS）、Notion API、Google Sheets、Python、LINE BOT、SATOプリンタ、Slack通知など</t>
   </si>
 </sst>
 </file>
@@ -495,12 +498,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2ED46DB-0EBD-4583-9EB3-25C3AD9387A5}">
-  <dimension ref="A1:B23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1368C6F3-2A74-4490-B0E8-1A908EC162C7}">
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="42.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="124.796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -623,7 +630,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>24</v>
@@ -631,6 +638,9 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
         <v>25</v>
       </c>
     </row>
@@ -638,40 +648,45 @@
       <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
         <v>28</v>
-      </c>
-      <c r="B20" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
         <v>30</v>
-      </c>
-      <c r="B21" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
         <v>32</v>
-      </c>
-      <c r="B22" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
         <v>34</v>
       </c>
-      <c r="B23" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
         <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>